<commit_message>
Added some of the dev tools to fedora-29, fixed a typo in run.sh
</commit_message>
<xml_diff>
--- a/compatibility-sheet.xlsx
+++ b/compatibility-sheet.xlsx
@@ -375,12 +375,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -452,11 +452,11 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="11.52"/>
@@ -495,7 +495,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="L2" s="2" t="s">
@@ -603,7 +603,7 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
     </row>
@@ -925,7 +925,7 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
+      <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="4"/>
     </row>
@@ -936,7 +936,7 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="3"/>
+      <c r="E41" s="2"/>
       <c r="F41" s="3"/>
       <c r="G41" s="4" t="s">
         <v>50</v>
@@ -949,7 +949,7 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="3"/>
+      <c r="E42" s="2"/>
       <c r="F42" s="3"/>
       <c r="G42" s="4"/>
     </row>
@@ -960,7 +960,7 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="3"/>
+      <c r="E43" s="2"/>
       <c r="F43" s="3"/>
       <c r="G43" s="4"/>
     </row>
@@ -971,7 +971,7 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="3"/>
+      <c r="E44" s="2"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
@@ -982,7 +982,7 @@
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="3"/>
+      <c r="E45" s="2"/>
       <c r="F45" s="3"/>
       <c r="G45" s="4"/>
     </row>
@@ -993,7 +993,7 @@
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="3"/>
+      <c r="E46" s="2"/>
       <c r="F46" s="3"/>
       <c r="G46" s="4"/>
     </row>
@@ -1026,7 +1026,7 @@
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="3"/>
+      <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
@@ -1037,7 +1037,7 @@
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="3"/>
+      <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
@@ -1048,7 +1048,7 @@
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="3"/>
+      <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
@@ -1059,7 +1059,7 @@
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="3"/>
+      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="3" t="s">
         <v>62</v>
@@ -1083,7 +1083,7 @@
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="3"/>
+      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
@@ -1094,7 +1094,7 @@
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="3"/>
+      <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>

</xml_diff>

<commit_message>
Removed Windows from .sh files
</commit_message>
<xml_diff>
--- a/compatibility-sheet.xlsx
+++ b/compatibility-sheet.xlsx
@@ -452,8 +452,8 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -614,7 +614,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added packagekit-qt5 to kde-plasma and added kde cleaner scripts on Arch
</commit_message>
<xml_diff>
--- a/compatibility-sheet.xlsx
+++ b/compatibility-sheet.xlsx
@@ -375,12 +375,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -453,7 +453,7 @@
   <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E57" activeCellId="0" sqref="E57"/>
+      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -600,7 +600,7 @@
       <c r="A11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
@@ -1105,7 +1105,7 @@
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="3"/>
+      <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
@@ -1116,7 +1116,7 @@
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="3"/>
+      <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
@@ -1127,7 +1127,7 @@
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="3"/>
+      <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
     </row>
@@ -1138,7 +1138,7 @@
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="3"/>
+      <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
@@ -1149,7 +1149,7 @@
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="3"/>
+      <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2" t="s">
         <v>71</v>
@@ -1162,7 +1162,7 @@
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="3"/>
+      <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
@@ -1173,7 +1173,7 @@
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="3"/>
+      <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
@@ -1184,7 +1184,7 @@
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="3"/>
+      <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
     </row>

</xml_diff>

<commit_message>
OS, user and hostname detection added, some refactoring
</commit_message>
<xml_diff>
--- a/compatibility-sheet.xlsx
+++ b/compatibility-sheet.xlsx
@@ -375,12 +375,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -452,8 +452,8 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E56" activeCellId="0" sqref="E56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1206,7 +1206,7 @@
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="3"/>
+      <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>

</xml_diff>